<commit_message>
added rail track lines, updated registered car statistics
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_coal_NRG_CB_SFFM.xlsx
+++ b/data/data_raw/eurostat/AT_coal_NRG_CB_SFFM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:GR50"/>
+  <dimension ref="A1:GS50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1429,6 +1429,11 @@
           <t>2024-02</t>
         </is>
       </c>
+      <c r="GS1" s="1" t="inlineStr">
+        <is>
+          <t>2024-03</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2038,7 +2043,10 @@
       <c r="GQ2" t="n">
         <v>0</v>
       </c>
-      <c r="GR2" t="inlineStr"/>
+      <c r="GR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2648,7 +2656,10 @@
       <c r="GQ3" t="n">
         <v>0</v>
       </c>
-      <c r="GR3" t="inlineStr"/>
+      <c r="GR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -3256,9 +3267,12 @@
         <v>161.937</v>
       </c>
       <c r="GQ4" t="n">
-        <v>194.417</v>
-      </c>
-      <c r="GR4" t="inlineStr"/>
+        <v>226.934</v>
+      </c>
+      <c r="GR4" t="n">
+        <v>202.213</v>
+      </c>
+      <c r="GS4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -3650,9 +3664,12 @@
         <v>73.46899999999999</v>
       </c>
       <c r="GQ5" t="n">
-        <v>89.584</v>
-      </c>
-      <c r="GR5" t="inlineStr"/>
+        <v>104.567</v>
+      </c>
+      <c r="GR5" t="n">
+        <v>96.98699999999999</v>
+      </c>
+      <c r="GS5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -4262,7 +4279,10 @@
       <c r="GQ6" t="n">
         <v>0</v>
       </c>
-      <c r="GR6" t="inlineStr"/>
+      <c r="GR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -4872,7 +4892,10 @@
       <c r="GQ7" t="n">
         <v>274.676</v>
       </c>
-      <c r="GR7" t="inlineStr"/>
+      <c r="GR7" t="n">
+        <v>279.399</v>
+      </c>
+      <c r="GS7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -5480,9 +5503,12 @@
         <v>274.676</v>
       </c>
       <c r="GQ8" t="n">
-        <v>262.828</v>
-      </c>
-      <c r="GR8" t="inlineStr"/>
+        <v>279.399</v>
+      </c>
+      <c r="GR8" t="n">
+        <v>278.357</v>
+      </c>
+      <c r="GS8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -6090,9 +6116,12 @@
         <v>49.735</v>
       </c>
       <c r="GQ9" t="n">
-        <v>11.848</v>
-      </c>
-      <c r="GR9" t="inlineStr"/>
+        <v>-4.722</v>
+      </c>
+      <c r="GR9" t="n">
+        <v>1.041</v>
+      </c>
+      <c r="GS9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -6700,9 +6729,12 @@
         <v>211.672</v>
       </c>
       <c r="GQ10" t="n">
-        <v>206.265</v>
-      </c>
-      <c r="GR10" t="inlineStr"/>
+        <v>222.212</v>
+      </c>
+      <c r="GR10" t="n">
+        <v>203.254</v>
+      </c>
+      <c r="GS10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -7094,9 +7126,12 @@
         <v>208.935</v>
       </c>
       <c r="GQ11" t="n">
-        <v>205.498</v>
-      </c>
-      <c r="GR11" t="inlineStr"/>
+        <v>223.412</v>
+      </c>
+      <c r="GR11" t="n">
+        <v>204.394</v>
+      </c>
+      <c r="GS11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -7706,7 +7741,10 @@
       <c r="GQ12" t="n">
         <v>0</v>
       </c>
-      <c r="GR12" t="inlineStr"/>
+      <c r="GR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -8316,7 +8354,10 @@
       <c r="GQ13" t="n">
         <v>147.532</v>
       </c>
-      <c r="GR13" t="inlineStr"/>
+      <c r="GR13" t="n">
+        <v>139.323</v>
+      </c>
+      <c r="GS13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -8924,9 +8965,12 @@
         <v>61.991</v>
       </c>
       <c r="GQ14" t="n">
-        <v>56.966</v>
-      </c>
-      <c r="GR14" t="inlineStr"/>
+        <v>74.88</v>
+      </c>
+      <c r="GR14" t="n">
+        <v>64.071</v>
+      </c>
+      <c r="GS14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -9318,9 +9362,12 @@
         <v>44.991</v>
       </c>
       <c r="GQ15" t="n">
-        <v>52.966</v>
-      </c>
-      <c r="GR15" t="inlineStr"/>
+        <v>70.88</v>
+      </c>
+      <c r="GR15" t="n">
+        <v>60.071</v>
+      </c>
+      <c r="GS15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -9930,7 +9977,10 @@
       <c r="GQ16" t="n">
         <v>1</v>
       </c>
-      <c r="GR16" t="inlineStr"/>
+      <c r="GR16" t="n">
+        <v>1</v>
+      </c>
+      <c r="GS16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -10322,9 +10372,12 @@
         <v>2.737</v>
       </c>
       <c r="GQ17" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="GR17" t="inlineStr"/>
+        <v>-1.2</v>
+      </c>
+      <c r="GR17" t="n">
+        <v>-1.14</v>
+      </c>
+      <c r="GS17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -10934,7 +10987,10 @@
       <c r="GQ18" t="n">
         <v>0</v>
       </c>
-      <c r="GR18" t="inlineStr"/>
+      <c r="GR18" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -11544,7 +11600,10 @@
       <c r="GQ19" t="n">
         <v>5.291</v>
       </c>
-      <c r="GR19" t="inlineStr"/>
+      <c r="GR19" t="n">
+        <v>0.766</v>
+      </c>
+      <c r="GS19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -12154,7 +12213,10 @@
       <c r="GQ20" t="n">
         <v>0</v>
       </c>
-      <c r="GR20" t="inlineStr"/>
+      <c r="GR20" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -12764,7 +12826,10 @@
       <c r="GQ21" t="n">
         <v>0</v>
       </c>
-      <c r="GR21" t="inlineStr"/>
+      <c r="GR21" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -13374,7 +13439,10 @@
       <c r="GQ22" t="n">
         <v>0</v>
       </c>
-      <c r="GR22" t="inlineStr"/>
+      <c r="GR22" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -13984,7 +14052,10 @@
       <c r="GQ23" t="n">
         <v>0</v>
       </c>
-      <c r="GR23" t="inlineStr"/>
+      <c r="GR23" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -14594,7 +14665,10 @@
       <c r="GQ24" t="n">
         <v>5.291</v>
       </c>
-      <c r="GR24" t="inlineStr"/>
+      <c r="GR24" t="n">
+        <v>0.766</v>
+      </c>
+      <c r="GS24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -15204,7 +15278,10 @@
       <c r="GQ25" t="n">
         <v>0</v>
       </c>
-      <c r="GR25" t="inlineStr"/>
+      <c r="GR25" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -15814,7 +15891,10 @@
       <c r="GQ26" t="n">
         <v>108.492</v>
       </c>
-      <c r="GR26" t="inlineStr"/>
+      <c r="GR26" t="n">
+        <v>96.321</v>
+      </c>
+      <c r="GS26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -16424,7 +16504,10 @@
       <c r="GQ27" t="n">
         <v>93.84</v>
       </c>
-      <c r="GR27" t="inlineStr"/>
+      <c r="GR27" t="n">
+        <v>108.974</v>
+      </c>
+      <c r="GS27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -16818,7 +16901,10 @@
       <c r="GQ28" t="n">
         <v>0</v>
       </c>
-      <c r="GR28" t="inlineStr"/>
+      <c r="GR28" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -17428,7 +17514,10 @@
       <c r="GQ29" t="n">
         <v>0</v>
       </c>
-      <c r="GR29" t="inlineStr"/>
+      <c r="GR29" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -18038,7 +18127,10 @@
       <c r="GQ30" t="n">
         <v>45.457</v>
       </c>
-      <c r="GR30" t="inlineStr"/>
+      <c r="GR30" t="n">
+        <v>38.412</v>
+      </c>
+      <c r="GS30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -18648,7 +18740,10 @@
       <c r="GQ31" t="n">
         <v>38.412</v>
       </c>
-      <c r="GR31" t="inlineStr"/>
+      <c r="GR31" t="n">
+        <v>55.634</v>
+      </c>
+      <c r="GS31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -19258,7 +19353,10 @@
       <c r="GQ32" t="n">
         <v>7.045</v>
       </c>
-      <c r="GR32" t="inlineStr"/>
+      <c r="GR32" t="n">
+        <v>-17.222</v>
+      </c>
+      <c r="GS32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -19868,7 +19966,10 @@
       <c r="GQ33" t="n">
         <v>209.377</v>
       </c>
-      <c r="GR33" t="inlineStr"/>
+      <c r="GR33" t="n">
+        <v>188.073</v>
+      </c>
+      <c r="GS33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -20478,7 +20579,10 @@
       <c r="GQ34" t="n">
         <v>196.074</v>
       </c>
-      <c r="GR34" t="inlineStr"/>
+      <c r="GR34" t="n">
+        <v>173.34</v>
+      </c>
+      <c r="GS34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -21088,7 +21192,10 @@
       <c r="GQ35" t="n">
         <v>0</v>
       </c>
-      <c r="GR35" t="inlineStr"/>
+      <c r="GR35" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -21698,7 +21805,10 @@
       <c r="GQ36" t="n">
         <v>0</v>
       </c>
-      <c r="GR36" t="inlineStr"/>
+      <c r="GR36" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -22308,7 +22418,10 @@
       <c r="GQ37" t="n">
         <v>0</v>
       </c>
-      <c r="GR37" t="inlineStr"/>
+      <c r="GR37" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -22749,6 +22862,7 @@
       <c r="GP38" t="inlineStr"/>
       <c r="GQ38" t="inlineStr"/>
       <c r="GR38" t="inlineStr"/>
+      <c r="GS38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -23189,6 +23303,7 @@
       <c r="GP39" t="inlineStr"/>
       <c r="GQ39" t="inlineStr"/>
       <c r="GR39" t="inlineStr"/>
+      <c r="GS39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -23798,7 +23913,10 @@
       <c r="GQ40" t="n">
         <v>0</v>
       </c>
-      <c r="GR40" t="inlineStr"/>
+      <c r="GR40" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -24408,7 +24526,10 @@
       <c r="GQ41" t="n">
         <v>0</v>
       </c>
-      <c r="GR41" t="inlineStr"/>
+      <c r="GR41" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -25018,7 +25139,10 @@
       <c r="GQ42" t="n">
         <v>0</v>
       </c>
-      <c r="GR42" t="inlineStr"/>
+      <c r="GR42" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -25412,7 +25536,10 @@
       <c r="GQ43" t="n">
         <v>0</v>
       </c>
-      <c r="GR43" t="inlineStr"/>
+      <c r="GR43" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -25806,7 +25933,10 @@
       <c r="GQ44" t="n">
         <v>0</v>
       </c>
-      <c r="GR44" t="inlineStr"/>
+      <c r="GR44" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -26200,7 +26330,10 @@
       <c r="GQ45" t="n">
         <v>0</v>
       </c>
-      <c r="GR45" t="inlineStr"/>
+      <c r="GR45" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -26594,7 +26727,10 @@
       <c r="GQ46" t="n">
         <v>0</v>
       </c>
-      <c r="GR46" t="inlineStr"/>
+      <c r="GR46" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -26988,7 +27124,10 @@
       <c r="GQ47" t="n">
         <v>0</v>
       </c>
-      <c r="GR47" t="inlineStr"/>
+      <c r="GR47" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -27382,7 +27521,10 @@
       <c r="GQ48" t="n">
         <v>0</v>
       </c>
-      <c r="GR48" t="inlineStr"/>
+      <c r="GR48" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -27776,7 +27918,10 @@
       <c r="GQ49" t="n">
         <v>0</v>
       </c>
-      <c r="GR49" t="inlineStr"/>
+      <c r="GR49" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -28170,7 +28315,10 @@
       <c r="GQ50" t="n">
         <v>0</v>
       </c>
-      <c r="GR50" t="inlineStr"/>
+      <c r="GR50" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add lulucf and uba data 2023
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_coal_NRG_CB_SFFM.xlsx
+++ b/data/data_raw/eurostat/AT_coal_NRG_CB_SFFM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:GZ50"/>
+  <dimension ref="A1:HA50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1469,6 +1469,11 @@
           <t>2024-10</t>
         </is>
       </c>
+      <c r="HA1" s="1" t="inlineStr">
+        <is>
+          <t>2024-11</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2103,6 +2108,7 @@
         <v>0</v>
       </c>
       <c r="GZ2" t="inlineStr"/>
+      <c r="HA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2737,6 +2743,7 @@
         <v>0</v>
       </c>
       <c r="GZ3" t="inlineStr"/>
+      <c r="HA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -3371,6 +3378,7 @@
         <v>148.218</v>
       </c>
       <c r="GZ4" t="inlineStr"/>
+      <c r="HA4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -3789,6 +3797,7 @@
         <v>88.17700000000001</v>
       </c>
       <c r="GZ5" t="inlineStr"/>
+      <c r="HA5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -4423,6 +4432,7 @@
         <v>0</v>
       </c>
       <c r="GZ6" t="inlineStr"/>
+      <c r="HA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -5057,6 +5067,7 @@
         <v>216.033</v>
       </c>
       <c r="GZ7" t="inlineStr"/>
+      <c r="HA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -5691,6 +5702,7 @@
         <v>178.356</v>
       </c>
       <c r="GZ8" t="inlineStr"/>
+      <c r="HA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -6325,6 +6337,7 @@
         <v>37.677</v>
       </c>
       <c r="GZ9" t="inlineStr"/>
+      <c r="HA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -6959,6 +6972,7 @@
         <v>185.896</v>
       </c>
       <c r="GZ10" t="inlineStr"/>
+      <c r="HA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -7377,6 +7391,7 @@
         <v>187.374</v>
       </c>
       <c r="GZ11" t="inlineStr"/>
+      <c r="HA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -8011,6 +8026,7 @@
         <v>0</v>
       </c>
       <c r="GZ12" t="inlineStr"/>
+      <c r="HA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -8645,6 +8661,7 @@
         <v>143.359</v>
       </c>
       <c r="GZ13" t="inlineStr"/>
+      <c r="HA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -9279,6 +9296,7 @@
         <v>43.015</v>
       </c>
       <c r="GZ14" t="inlineStr"/>
+      <c r="HA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -9697,6 +9715,7 @@
         <v>38.015</v>
       </c>
       <c r="GZ15" t="inlineStr"/>
+      <c r="HA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -10331,6 +10350,7 @@
         <v>1</v>
       </c>
       <c r="GZ16" t="inlineStr"/>
+      <c r="HA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -10749,6 +10769,7 @@
         <v>-1.479</v>
       </c>
       <c r="GZ17" t="inlineStr"/>
+      <c r="HA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -11383,6 +11404,7 @@
         <v>0</v>
       </c>
       <c r="GZ18" t="inlineStr"/>
+      <c r="HA18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -12017,6 +12039,7 @@
         <v>5.227</v>
       </c>
       <c r="GZ19" t="inlineStr"/>
+      <c r="HA19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -12651,6 +12674,7 @@
         <v>0</v>
       </c>
       <c r="GZ20" t="inlineStr"/>
+      <c r="HA20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -13285,6 +13309,7 @@
         <v>0</v>
       </c>
       <c r="GZ21" t="inlineStr"/>
+      <c r="HA21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -13919,6 +13944,7 @@
         <v>0</v>
       </c>
       <c r="GZ22" t="inlineStr"/>
+      <c r="HA22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -14553,6 +14579,7 @@
         <v>0</v>
       </c>
       <c r="GZ23" t="inlineStr"/>
+      <c r="HA23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -15187,6 +15214,7 @@
         <v>5.227</v>
       </c>
       <c r="GZ24" t="inlineStr"/>
+      <c r="HA24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -15821,6 +15849,7 @@
         <v>0</v>
       </c>
       <c r="GZ25" t="inlineStr"/>
+      <c r="HA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -16455,6 +16484,7 @@
         <v>104.138</v>
       </c>
       <c r="GZ26" t="inlineStr"/>
+      <c r="HA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -17089,6 +17119,7 @@
         <v>28.113</v>
       </c>
       <c r="GZ27" t="inlineStr"/>
+      <c r="HA27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -17507,6 +17538,7 @@
         <v>0</v>
       </c>
       <c r="GZ28" t="inlineStr"/>
+      <c r="HA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -18141,6 +18173,7 @@
         <v>0</v>
       </c>
       <c r="GZ29" t="inlineStr"/>
+      <c r="HA29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -18775,6 +18808,7 @@
         <v>88.014</v>
       </c>
       <c r="GZ30" t="inlineStr"/>
+      <c r="HA30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -19409,6 +19443,7 @@
         <v>78.086</v>
       </c>
       <c r="GZ31" t="inlineStr"/>
+      <c r="HA31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -20043,6 +20078,7 @@
         <v>9.929</v>
       </c>
       <c r="GZ32" t="inlineStr"/>
+      <c r="HA32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -20677,6 +20713,7 @@
         <v>142.179</v>
       </c>
       <c r="GZ33" t="inlineStr"/>
+      <c r="HA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -21311,6 +21348,7 @@
         <v>136.719</v>
       </c>
       <c r="GZ34" t="inlineStr"/>
+      <c r="HA34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -21945,6 +21983,7 @@
         <v>0</v>
       </c>
       <c r="GZ35" t="inlineStr"/>
+      <c r="HA35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -22579,6 +22618,7 @@
         <v>0</v>
       </c>
       <c r="GZ36" t="inlineStr"/>
+      <c r="HA36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -23213,6 +23253,7 @@
         <v>0</v>
       </c>
       <c r="GZ37" t="inlineStr"/>
+      <c r="HA37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -23661,6 +23702,7 @@
       <c r="GX38" t="inlineStr"/>
       <c r="GY38" t="inlineStr"/>
       <c r="GZ38" t="inlineStr"/>
+      <c r="HA38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -24109,6 +24151,7 @@
       <c r="GX39" t="inlineStr"/>
       <c r="GY39" t="inlineStr"/>
       <c r="GZ39" t="inlineStr"/>
+      <c r="HA39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -24743,6 +24786,7 @@
         <v>0</v>
       </c>
       <c r="GZ40" t="inlineStr"/>
+      <c r="HA40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -25377,6 +25421,7 @@
         <v>0</v>
       </c>
       <c r="GZ41" t="inlineStr"/>
+      <c r="HA41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -26011,6 +26056,7 @@
         <v>0</v>
       </c>
       <c r="GZ42" t="inlineStr"/>
+      <c r="HA42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -26429,6 +26475,7 @@
         <v>0</v>
       </c>
       <c r="GZ43" t="inlineStr"/>
+      <c r="HA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -26847,6 +26894,7 @@
         <v>0</v>
       </c>
       <c r="GZ44" t="inlineStr"/>
+      <c r="HA44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -27265,6 +27313,7 @@
         <v>0</v>
       </c>
       <c r="GZ45" t="inlineStr"/>
+      <c r="HA45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -27683,6 +27732,7 @@
         <v>0</v>
       </c>
       <c r="GZ46" t="inlineStr"/>
+      <c r="HA46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -28101,6 +28151,7 @@
         <v>0</v>
       </c>
       <c r="GZ47" t="inlineStr"/>
+      <c r="HA47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -28519,6 +28570,7 @@
         <v>0</v>
       </c>
       <c r="GZ48" t="inlineStr"/>
+      <c r="HA48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -28937,6 +28989,7 @@
         <v>0</v>
       </c>
       <c r="GZ49" t="inlineStr"/>
+      <c r="HA49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -29355,6 +29408,7 @@
         <v>0</v>
       </c>
       <c r="GZ50" t="inlineStr"/>
+      <c r="HA50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>